<commit_message>
Arreglo de calculo, calculo pasa de ser de 12h a 24h, pequeños cambios a GUI, mejoramiento de la interfaz
</commit_message>
<xml_diff>
--- a/dist/prestamos.xlsx
+++ b/dist/prestamos.xlsx
@@ -558,11 +558,11 @@
         <v>500</v>
       </c>
       <c r="G3" t="n">
-        <v>3900</v>
+        <v>0</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>ACTIVO</t>
+          <t>CERRADO</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">

</xml_diff>